<commit_message>
commit de avance de datos, limpieza marzo 2024
</commit_message>
<xml_diff>
--- a/tesis_doctorado/datav2023/base_datosausentes.xlsx
+++ b/tesis_doctorado/datav2023/base_datosausentes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="285">
   <si>
     <t xml:space="preserve">ncat_eleccion</t>
   </si>
@@ -785,6 +785,96 @@
   </si>
   <si>
     <t xml:space="preserve">https://es.wikipedia.org/wiki/Elecci%C3%B3n_presidencial_de_El_Salvador_de_2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://es.wikipedia.org/wiki/Elecciones_generales_de_Guatemala_de_2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carlos Pineda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SU CANDIDATURA FUE ANULADA. https://es.wikipedia.org/wiki/Elecciones_generales_de_Guatemala_de_2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rudy Guzmán</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manuel Villacorta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isaac Farchi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rafael Espada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Almícar Pop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://es.wikipedia.org/wiki/Elecciones_generales_de_Guatemala_de_2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amílcar Rivera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://es.wikipedia.org/wiki/Elecciones_generales_de_Guatemala_de_2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bernardo Arévalo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://es.wikipedia.org/wiki/Elecciones_generales_de_Guatemala_de_2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edmond Mulet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://es.wikipedia.org/wiki/Elecciones_generales_de_Guatemala_de_2027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giulio Talamonti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://es.wikipedia.org/wiki/Elecciones_generales_de_Guatemala_de_2028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Julio Rivera Clavería</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://es.wikipedia.org/wiki/Elecciones_generales_de_Guatemala_de_2029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luis Lam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://es.wikipedia.org/wiki/Elecciones_generales_de_Guatemala_de_2030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manuel Conde Orellana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://es.wikipedia.org/wiki/Elecciones_generales_de_Guatemala_de_2031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ricardo Sagastume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://es.wikipedia.org/wiki/Elecciones_generales_de_Guatemala_de_2032</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rudio Lecsan Mérida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://es.wikipedia.org/wiki/Elecciones_generales_de_Guatemala_de_2033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://es.wikipedia.org/wiki/Elecciones_generales_de_Guatemala_de_2034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samuel Morales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://es.wikipedia.org/wiki/Elecciones_generales_de_Guatemala_de_2035</t>
   </si>
 </sst>
 </file>
@@ -907,7 +997,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -949,10 +1039,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1034,10 +1120,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G168"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C50" activeCellId="0" sqref="C50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A127" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E143" activeCellId="0" sqref="E143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3624,7 +3710,7 @@
       <c r="F122" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G122" s="11" t="s">
+      <c r="G122" s="7" t="s">
         <v>187</v>
       </c>
     </row>
@@ -4022,7 +4108,9 @@
       <c r="C141" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="D141" s="7"/>
+      <c r="D141" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="G141" s="7" t="s">
         <v>211</v>
       </c>
@@ -4037,6 +4125,9 @@
       <c r="C142" s="10" t="s">
         <v>212</v>
       </c>
+      <c r="D142" s="0" t="s">
+        <v>26</v>
+      </c>
       <c r="G142" s="7" t="s">
         <v>213</v>
       </c>
@@ -4621,11 +4712,455 @@
         <v>254</v>
       </c>
     </row>
+    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="0" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B169" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C169" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="D169" s="0" t="n">
+        <v>6.59</v>
+      </c>
+      <c r="E169" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F169" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G169" s="0" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="0" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B170" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C170" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="D170" s="0" t="n">
+        <v>15.97</v>
+      </c>
+      <c r="E170" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F170" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G170" s="0" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="0" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B171" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C171" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="D171" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E171" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F171" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G171" s="0" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="0" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B172" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C172" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="D172" s="0" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="E172" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F172" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G172" s="0" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="0" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B173" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C173" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="D173" s="0" t="n">
+        <v>4.26</v>
+      </c>
+      <c r="E173" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F173" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G173" s="0" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="0" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B174" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C174" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="D174" s="0" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="E174" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F174" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G174" s="0" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="0" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B175" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C175" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="D175" s="0" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="E175" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F175" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G175" s="0" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="0" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B176" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C176" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="D176" s="0" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="E176" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F176" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G176" s="0" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="0" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B177" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C177" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="D177" s="0" t="n">
+        <v>2.48</v>
+      </c>
+      <c r="E177" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F177" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G177" s="0" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="0" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B178" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C178" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="D178" s="0" t="n">
+        <v>11.74</v>
+      </c>
+      <c r="E178" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F178" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G178" s="0" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="0" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B179" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C179" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="D179" s="0" t="n">
+        <v>6.65</v>
+      </c>
+      <c r="E179" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F179" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G179" s="0" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="0" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B180" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C180" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="D180" s="0" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="E180" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F180" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G180" s="0" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="0" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B181" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C181" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="D181" s="0" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="E181" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F181" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G181" s="0" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="0" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B182" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C182" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="D182" s="0" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="E182" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F182" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G182" s="0" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="0" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B183" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C183" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="D183" s="0" t="n">
+        <v>7.85</v>
+      </c>
+      <c r="E183" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F183" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G183" s="0" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="0" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B184" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C184" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="D184" s="0" t="n">
+        <v>1.41</v>
+      </c>
+      <c r="E184" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F184" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G184" s="0" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="0" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B185" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C185" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="D185" s="0" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="E185" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F185" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G185" s="0" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="0" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B186" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C186" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="D186" s="0" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="E186" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F186" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G186" s="0" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="0" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B187" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C187" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="D187" s="0" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="E187" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F187" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G187" s="0" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" display="https://es.wikipedia.org/wiki/Elecciones_generales_de_Brasil_de_2022"/>
     <hyperlink ref="G3" r:id="rId2" display="https://es.wikipedia.org/wiki/Elecciones_generales_de_Brasil_de_2022"/>
-    <hyperlink ref="G20" r:id="rId3" location="Resultados" display="https://es.wikipedia.org/wiki/Elecciones_generales_de_Costa_Rica_de_2022#Resultados"/>
+    <hyperlink ref="G20" r:id="rId3" location="Resultados" display="Candidatura denegada por TSE.  https://es.wikipedia.org/wiki/Elecciones_generales_de_Costa_Rica_de_2022#Resultados"/>
     <hyperlink ref="G38" r:id="rId4" display="https://pdba.georgetown.edu/"/>
     <hyperlink ref="G39" r:id="rId5" display="https://pdba.georgetown.edu/"/>
     <hyperlink ref="G40" r:id="rId6" display="https://pdba.georgetown.edu/"/>
@@ -4740,6 +5275,7 @@
     <hyperlink ref="G166" r:id="rId115" display="https://es.wikipedia.org/wiki/Elecciones_generales_de_la_Rep%C3%BAblica_Dominicana_de_2016"/>
     <hyperlink ref="G167" r:id="rId116" display="https://pdba.georgetown.edu/Elecdata/ElSal/pre99.html"/>
     <hyperlink ref="G168" r:id="rId117" display="https://es.wikipedia.org/wiki/Elecci%C3%B3n_presidencial_de_El_Salvador_de_2019"/>
+    <hyperlink ref="G171" r:id="rId118" display="SU CANDIDATURA FUE ANULADA. https://es.wikipedia.org/wiki/Elecciones_generales_de_Guatemala_de_2023"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>